<commit_message>
Updates to cleanCGM and CGM dictionary. Changed full expected wear to be able to be specified in dictionary with default values added. expcted wear can still be specified as shorter in the function argument. In addition changed gaptesting to be more generic based on the interval of the data to avoid having to specify interval for specific CGMs. Changed outputs to be csv format.
</commit_message>
<xml_diff>
--- a/inst/extdata/cgmvariable_dictionary.xlsx
+++ b/inst/extdata/cgmvariable_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/CGMprocessing/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78DF54BE-E327-5642-8169-1813572EB3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C970C6-FF6B-F242-8B52-F30FC1EE4729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="1780" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>old_vars</t>
   </si>
@@ -100,13 +100,16 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>expectedwear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,16 +129,29 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -143,13 +159,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,15 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4196811C-C02D-BF4D-A15B-96DBE2D70C76}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -485,6 +519,9 @@
       <c r="C1" t="s">
         <v>13</v>
       </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -496,6 +533,9 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -507,6 +547,9 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -518,6 +561,9 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -529,6 +575,9 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -540,6 +589,9 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -551,6 +603,9 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -562,6 +617,9 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -573,6 +631,9 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -584,6 +645,9 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -595,6 +659,9 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -605,6 +672,9 @@
       </c>
       <c r="C12" t="s">
         <v>23</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -629,6 +699,12 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Updates to cleanCGM and CGM dictionary. Changed full expected wear to be able to be specified in dictionary with default values added. expcted wear can still be specified as shorter in the function argument. In addition changed gaptesting to be more generic based on the interval of the data to avoid having to specify interval for specific CGMs.
</commit_message>
<xml_diff>
--- a/inst/extdata/cgmvariable_dictionary.xlsx
+++ b/inst/extdata/cgmvariable_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/CGMprocessing/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78DF54BE-E327-5642-8169-1813572EB3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C970C6-FF6B-F242-8B52-F30FC1EE4729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="1780" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>old_vars</t>
   </si>
@@ -100,13 +100,16 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>expectedwear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,16 +129,29 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -143,13 +159,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,15 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4196811C-C02D-BF4D-A15B-96DBE2D70C76}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -485,6 +519,9 @@
       <c r="C1" t="s">
         <v>13</v>
       </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -496,6 +533,9 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -507,6 +547,9 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -518,6 +561,9 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -529,6 +575,9 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -540,6 +589,9 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -551,6 +603,9 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -562,6 +617,9 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -573,6 +631,9 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -584,6 +645,9 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -595,6 +659,9 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -605,6 +672,9 @@
       </c>
       <c r="C12" t="s">
         <v>23</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -629,6 +699,12 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Updated rmd and cleanCGM
</commit_message>
<xml_diff>
--- a/inst/extdata/cgmvariable_dictionary.xlsx
+++ b/inst/extdata/cgmvariable_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/CGMprocessing/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C970C6-FF6B-F242-8B52-F30FC1EE4729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D13AE8-73FD-4B42-9244-7F634ADD5CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="1780" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
   </bookViews>
@@ -23,12 +23,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>old_vars</t>
   </si>
@@ -54,21 +65,12 @@
     <t>recordtype</t>
   </si>
   <si>
-    <t>Device</t>
-  </si>
-  <si>
     <t>Serial Number</t>
   </si>
   <si>
     <t>Device Timestamp</t>
   </si>
   <si>
-    <t>Historic Glucose mmol/L</t>
-  </si>
-  <si>
-    <t>Scan Glucose mmol/L</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -102,7 +104,19 @@
     <t>other</t>
   </si>
   <si>
-    <t>expectedwear</t>
+    <t>sensor_lifetime</t>
+  </si>
+  <si>
+    <t>Record Type</t>
+  </si>
+  <si>
+    <t>scan_yn</t>
+  </si>
+  <si>
+    <t>Historic Glucose(mmol/L)</t>
+  </si>
+  <si>
+    <t>Scan Glucose(mmol/L)</t>
   </si>
 </sst>
 </file>
@@ -500,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4196811C-C02D-BF4D-A15B-96DBE2D70C76}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,10 +531,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -528,10 +542,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>14</v>
@@ -542,10 +556,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>14</v>
@@ -553,13 +567,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>14</v>
@@ -567,13 +581,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>14</v>
@@ -581,13 +595,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>14</v>
@@ -595,13 +609,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -609,13 +623,13 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -623,13 +637,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -637,13 +651,13 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -651,13 +665,13 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -671,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -691,13 +705,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>10</v>

</xml_diff>

<commit_message>
New version. Updated so pre-aggregated data from clincial trials can be handled. More updates to README.
</commit_message>
<xml_diff>
--- a/inst/extdata/cgmvariable_dictionary.xlsx
+++ b/inst/extdata/cgmvariable_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/CGMprocessing/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D13AE8-73FD-4B42-9244-7F634ADD5CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4820B7F3-EFC3-F642-A180-8F8E9AD67E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="1780" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
+    <workbookView xWindow="1400" yWindow="1200" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>device</t>
-  </si>
-  <si>
     <t>libre</t>
   </si>
   <si>
@@ -95,18 +89,9 @@
     <t>record_type</t>
   </si>
   <si>
-    <t>pt_id</t>
-  </si>
-  <si>
-    <t>device_dt_tm</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
-    <t>sensor_lifetime</t>
-  </si>
-  <si>
     <t>Record Type</t>
   </si>
   <si>
@@ -117,6 +102,21 @@
   </si>
   <si>
     <t>Scan Glucose(mmol/L)</t>
+  </si>
+  <si>
+    <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>GLUCOSE</t>
+  </si>
+  <si>
+    <t>ID_VISIT_DEVICEID</t>
+  </si>
+  <si>
+    <t>deviceid</t>
+  </si>
+  <si>
+    <t>expecteddaysofwear</t>
   </si>
 </sst>
 </file>
@@ -216,9 +216,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,7 +256,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -362,7 +362,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -504,7 +504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4196811C-C02D-BF4D-A15B-96DBE2D70C76}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,21 +531,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>14</v>
@@ -553,13 +553,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>14</v>
@@ -567,13 +567,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>14</v>
@@ -581,13 +581,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>14</v>
@@ -595,13 +595,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>14</v>
@@ -609,13 +609,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -623,13 +623,13 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -637,13 +637,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -651,44 +651,44 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -705,13 +705,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>10</v>

</xml_diff>

<commit_message>
updates to exercise_split, simplify sgm dictionary to dexcom from dexcomg6
</commit_message>
<xml_diff>
--- a/inst/extdata/cgmvariable_dictionary.xlsx
+++ b/inst/extdata/cgmvariable_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/CGMprocessing/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4820B7F3-EFC3-F642-A180-8F8E9AD67E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6531105-DA4D-2241-A048-731291C2D702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="1200" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Glucose Value (mmol/L)</t>
   </si>
   <si>
-    <t>dexcomg6</t>
-  </si>
-  <si>
     <t>record_type</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>expecteddaysofwear</t>
+  </si>
+  <si>
+    <t>dexcom</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +534,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -542,7 +542,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -581,10 +581,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -615,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -629,7 +629,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -640,10 +640,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -651,13 +651,13 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>14</v>
@@ -665,13 +665,13 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>14</v>
@@ -679,13 +679,13 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <v>14</v>
@@ -705,13 +705,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>10</v>

</xml_diff>

<commit_message>
edits to README and clairty of all functions
</commit_message>
<xml_diff>
--- a/inst/extdata/cgmvariable_dictionary.xlsx
+++ b/inst/extdata/cgmvariable_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/CGMprocessing/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6531105-DA4D-2241-A048-731291C2D702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CC06E0-E012-E442-B033-EFFBA9060E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1200" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
+    <workbookView xWindow="37460" yWindow="3000" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>old_vars</t>
   </si>
@@ -117,13 +117,19 @@
   </si>
   <si>
     <t>dexcom</t>
+  </si>
+  <si>
+    <t>Event Type</t>
+  </si>
+  <si>
+    <t>eventtype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,29 +149,16 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -173,31 +166,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4196811C-C02D-BF4D-A15B-96DBE2D70C76}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,7 +693,18 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Addition of parmater to cleanCGM function to enable user specified cgm dictionary, otherwise package cgm dictionary is used
</commit_message>
<xml_diff>
--- a/inst/extdata/cgmvariable_dictionary.xlsx
+++ b/inst/extdata/cgmvariable_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/CGMprocessing/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CC06E0-E012-E442-B033-EFFBA9060E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256E87B4-1B3C-CC4C-9076-A33C9B0FFE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37460" yWindow="3000" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>old_vars</t>
   </si>
@@ -56,12 +56,6 @@
     <t>sensorglucose</t>
   </si>
   <si>
-    <t>scanglucose</t>
-  </si>
-  <si>
-    <t>recordtype</t>
-  </si>
-  <si>
     <t>Serial Number</t>
   </si>
   <si>
@@ -83,22 +77,13 @@
     <t>Glucose Value (mmol/L)</t>
   </si>
   <si>
-    <t>record_type</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
     <t>Record Type</t>
   </si>
   <si>
-    <t>scan_yn</t>
-  </si>
-  <si>
     <t>Historic Glucose(mmol/L)</t>
-  </si>
-  <si>
-    <t>Scan Glucose(mmol/L)</t>
   </si>
   <si>
     <t>TIMESTAMP</t>
@@ -487,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4196811C-C02D-BF4D-A15B-96DBE2D70C76}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,21 +491,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>14</v>
@@ -528,13 +513,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>14</v>
@@ -542,13 +527,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>14</v>
@@ -556,41 +541,41 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
         <v>10</v>
-      </c>
-      <c r="D6">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -598,13 +583,13 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -612,13 +597,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -626,13 +611,13 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>14</v>
@@ -640,13 +625,13 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>14</v>
@@ -654,13 +639,13 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <v>14</v>
@@ -678,34 +663,6 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to libre dictionary
</commit_message>
<xml_diff>
--- a/inst/extdata/cgmvariable_dictionary.xlsx
+++ b/inst/extdata/cgmvariable_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicecarr/Desktop/CGMprocessing/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256E87B4-1B3C-CC4C-9076-A33C9B0FFE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406F0CC3-9AC9-764C-9783-914959BBE30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37460" yWindow="3000" windowWidth="20360" windowHeight="12040" xr2:uid="{95CED60D-52FF-9E44-B892-971B4CE0580C}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Record Type</t>
   </si>
   <si>
-    <t>Historic Glucose(mmol/L)</t>
-  </si>
-  <si>
     <t>TIMESTAMP</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>eventtype</t>
+  </si>
+  <si>
+    <t>Historic Glucose mmol/L</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,7 +494,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -544,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -558,10 +558,10 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -575,7 +575,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -589,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -597,13 +597,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -625,7 +625,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>

</xml_diff>